<commit_message>
feat: Added refactor version Fraga_Pinch_Method1
</commit_message>
<xml_diff>
--- a/tutorial/streams/AEStreamTable2.xlsx
+++ b/tutorial/streams/AEStreamTable2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nokman/git/PyPinch/tutorial/streams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B275EC-DD00-4444-96D1-F8E46DF6730D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375DEC8C-C68B-3142-86CB-EDDBBB24FC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Tout</t>
   </si>
   <si>
-    <t xml:space="preserve">T_diff </t>
-  </si>
-  <si>
     <t>Cp (kJ/kmol/K)</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>S37</t>
+  </si>
+  <si>
+    <t>T_diff</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -512,10 +512,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -524,10 +524,10 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>162.59865199999999</v>
@@ -548,10 +548,10 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>309.3176618</v>
@@ -573,10 +573,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>256</v>
@@ -597,10 +597,10 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>575.34732440000005</v>
@@ -622,10 +622,10 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
         <v>158.3520293</v>
@@ -646,10 +646,10 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>500</v>
@@ -670,10 +670,10 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
         <v>337.0182461</v>
@@ -694,10 +694,10 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2">
         <v>322</v>
@@ -719,10 +719,10 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1">
         <v>7.4976159999999998</v>
@@ -743,10 +743,10 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1">
         <v>215.71549999999999</v>
@@ -767,10 +767,10 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1">
         <v>196.1049419</v>
@@ -791,10 +791,10 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
         <v>125.9180805</v>
@@ -815,10 +815,10 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <v>30.641400000000001</v>
@@ -839,10 +839,10 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1">
         <v>79.933218260000004</v>
@@ -867,14 +867,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="dba03bd0-07eb-47bd-a862-a3b0372df2ff" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8b148402-c3d2-4106-8de5-94ce7d275064">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1095,21 +1093,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dba03bd0-07eb-47bd-a862-a3b0372df2ff" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8b148402-c3d2-4106-8de5-94ce7d275064">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38994224-EB57-455E-9FB3-99E183BC8079}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D609CD12-F426-44A9-A7AF-C7AEFEEB68B2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dba03bd0-07eb-47bd-a862-a3b0372df2ff"/>
-    <ds:schemaRef ds:uri="8b148402-c3d2-4106-8de5-94ce7d275064"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1134,9 +1131,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D609CD12-F426-44A9-A7AF-C7AEFEEB68B2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38994224-EB57-455E-9FB3-99E183BC8079}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dba03bd0-07eb-47bd-a862-a3b0372df2ff"/>
+    <ds:schemaRef ds:uri="8b148402-c3d2-4106-8de5-94ce7d275064"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>